<commit_message>
slight change in excel
</commit_message>
<xml_diff>
--- a/recipeCreationCMode.xlsx
+++ b/recipeCreationCMode.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Lattice\Desktop\ss\RecipeCreation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CB97D2D3-38F3-4DB9-961C-5ACD8EFA46D6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{59912A90-3F71-4078-A582-FE4C5A1C2D45}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-98" yWindow="-98" windowWidth="20715" windowHeight="13276" tabRatio="753" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1313,7 +1313,7 @@
   <dimension ref="A1:H96"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="84" zoomScaleNormal="84" workbookViewId="0">
-      <selection activeCell="H59" sqref="H59"/>
+      <selection activeCell="G8" sqref="G8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -1452,11 +1452,8 @@
       <c r="A6">
         <v>1.1000000000000001</v>
       </c>
-      <c r="B6" t="s">
-        <v>8</v>
-      </c>
       <c r="C6" t="s">
-        <v>20</v>
+        <v>26</v>
       </c>
       <c r="D6" t="s">
         <v>21</v>
@@ -1465,15 +1462,18 @@
         <v>12</v>
       </c>
       <c r="F6" t="s">
-        <v>25</v>
+        <v>28</v>
       </c>
       <c r="G6" t="s">
-        <v>13</v>
+        <v>22</v>
       </c>
       <c r="H6" s="7"/>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A7">
+        <v>1.2</v>
+      </c>
+      <c r="B7">
         <v>1.1000000000000001</v>
       </c>
       <c r="C7" t="s">
@@ -1482,39 +1482,39 @@
       <c r="D7" t="s">
         <v>21</v>
       </c>
-      <c r="E7" s="9" t="s">
-        <v>12</v>
-      </c>
-      <c r="F7" t="s">
-        <v>28</v>
-      </c>
-      <c r="G7" t="s">
-        <v>22</v>
-      </c>
-      <c r="H7" s="7"/>
+      <c r="E7" s="16" t="s">
+        <v>12</v>
+      </c>
+      <c r="F7" s="6" t="s">
+        <v>27</v>
+      </c>
+      <c r="G7" s="6" t="s">
+        <v>22</v>
+      </c>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A8">
-        <v>1.2</v>
-      </c>
-      <c r="B8">
-        <v>1.1000000000000001</v>
+        <v>1.1000000000000001</v>
+      </c>
+      <c r="B8" t="s">
+        <v>8</v>
       </c>
       <c r="C8" t="s">
-        <v>26</v>
+        <v>20</v>
       </c>
       <c r="D8" t="s">
         <v>21</v>
       </c>
-      <c r="E8" s="16" t="s">
-        <v>12</v>
-      </c>
-      <c r="F8" s="6" t="s">
-        <v>27</v>
-      </c>
-      <c r="G8" s="6" t="s">
-        <v>22</v>
-      </c>
+      <c r="E8" s="9" t="s">
+        <v>12</v>
+      </c>
+      <c r="F8" t="s">
+        <v>25</v>
+      </c>
+      <c r="G8" t="s">
+        <v>13</v>
+      </c>
+      <c r="H8" s="7"/>
     </row>
     <row r="9" spans="1:8" ht="28.5" x14ac:dyDescent="0.45">
       <c r="A9">
@@ -3575,7 +3575,7 @@
   <dimension ref="A1:H96"/>
   <sheetViews>
     <sheetView topLeftCell="A28" workbookViewId="0">
-      <selection activeCell="C68" sqref="C68"/>
+      <selection activeCell="A6" sqref="A6:XFD6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -5836,7 +5836,7 @@
   <dimension ref="A1:H96"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="J65" sqref="J65"/>
+      <selection activeCell="A6" sqref="A6:XFD6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -8097,7 +8097,7 @@
   <dimension ref="A1:H96"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A35" sqref="A35:XFD35"/>
+      <selection activeCell="A6" sqref="A6:XFD6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -10358,7 +10358,7 @@
   <dimension ref="A1:H96"/>
   <sheetViews>
     <sheetView zoomScale="86" zoomScaleNormal="86" workbookViewId="0">
-      <selection activeCell="C19" sqref="C19:C21"/>
+      <selection activeCell="G6" sqref="G6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -12619,7 +12619,7 @@
   <dimension ref="A1:J96"/>
   <sheetViews>
     <sheetView zoomScale="83" zoomScaleNormal="83" workbookViewId="0">
-      <selection activeCell="C19" sqref="C19:C21"/>
+      <selection activeCell="A6" sqref="A6:XFD6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -14881,7 +14881,7 @@
   <dimension ref="A1:H96"/>
   <sheetViews>
     <sheetView topLeftCell="A28" zoomScale="84" zoomScaleNormal="84" workbookViewId="0">
-      <selection activeCell="C55" sqref="C55:C59"/>
+      <selection activeCell="A6" sqref="A6:XFD6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -17142,7 +17142,7 @@
   <dimension ref="A1:H96"/>
   <sheetViews>
     <sheetView topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="J65" sqref="J65"/>
+      <selection activeCell="A6" sqref="A6:XFD6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -19403,7 +19403,7 @@
   <dimension ref="A1:H96"/>
   <sheetViews>
     <sheetView topLeftCell="A16" workbookViewId="0">
-      <selection activeCell="C19" sqref="C19:C21"/>
+      <selection activeCell="A6" sqref="A6:XFD6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -21664,7 +21664,7 @@
   <dimension ref="A1:H96"/>
   <sheetViews>
     <sheetView topLeftCell="A28" workbookViewId="0">
-      <selection activeCell="H59" sqref="H59"/>
+      <selection activeCell="A6" sqref="A6:XFD6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -23925,7 +23925,7 @@
   <dimension ref="A1:H96"/>
   <sheetViews>
     <sheetView topLeftCell="A64" workbookViewId="0">
-      <selection activeCell="H59" sqref="H59"/>
+      <selection activeCell="A6" sqref="A6:XFD6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -26186,7 +26186,7 @@
   <dimension ref="A1:H96"/>
   <sheetViews>
     <sheetView topLeftCell="A28" workbookViewId="0">
-      <selection activeCell="C19" sqref="C19:C21"/>
+      <selection activeCell="A6" sqref="A6:XFD6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>

</xml_diff>